<commit_message>
Exercise 1: Cleanse the Data + Add Derived Columns + Find the Highest and Lowest Temperatures
</commit_message>
<xml_diff>
--- a/1/DAT101x_Labfiles/Book1.xlsx
+++ b/1/DAT101x_Labfiles/Book1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="12">
   <si>
     <t>Date</t>
   </si>
@@ -51,6 +51,15 @@
   </si>
   <si>
     <t>Beach</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Total revenue</t>
   </si>
 </sst>
 </file>
@@ -93,7 +102,137 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FF9C0006"/>
+        </left>
+        <right style="thin">
+          <color rgb="FF9C0006"/>
+        </right>
+        <top style="thin">
+          <color rgb="FF9C0006"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF9C0006"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -110,17 +249,1092 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$A$1:$A$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$A$2:$A$32</c:f>
+              <c:strCache>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>7/1/2016</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7/2/2016</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7/3/2016</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7/4/2016</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7/5/2016</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7/6/2016</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7/7/2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7/8/2016</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7/9/2016</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7/10/2016</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7/11/2016</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7/12/2016</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7/13/2016</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>7/14/2016</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7/15/2016</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7/16/2016</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>7/17/2016</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7/18/2016</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7/19/2016</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7/20/2016</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7/21/2016</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7/22/2016</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7/23/2016</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7/24/2016</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7/25/2016</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7/26/2016</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>7/27/2016</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>7/28/2016</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>7/29/2016</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>7/30/2016</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7/31/2016</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$I$1:$I$32</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$I$2:$I$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>41.25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>69.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>52.25</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>57.25</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>59.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>70.5</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>56.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>51.75</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>65.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>95.5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>111.5</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>103.5</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>56.5</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>66.5</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>93.5</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>101.5</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>134.5</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>106.75</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>60.199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>55.65</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>58.099999999999994</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>50.75</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>43.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-13E3-4CBC-AE55-63C4C6F3A0CC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="706075136"/>
+        <c:axId val="706076448"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="706075136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="706076448"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="706076448"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="706075136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G32" totalsRowShown="0">
-  <autoFilter ref="A1:G32"/>
-  <tableColumns count="7">
-    <tableColumn id="1" name="Date" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I32" totalsRowShown="0">
+  <autoFilter ref="A1:I32"/>
+  <tableColumns count="9">
+    <tableColumn id="1" name="Date" dataDxfId="12"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="3" name="Lemon"/>
     <tableColumn id="4" name="Orange"/>
     <tableColumn id="5" name="Temperature"/>
     <tableColumn id="6" name="Leaflets"/>
     <tableColumn id="7" name="Price"/>
+    <tableColumn id="8" name="Sales" dataDxfId="11">
+      <calculatedColumnFormula>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" name="Revenue" dataDxfId="10">
+      <calculatedColumnFormula>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -389,10 +1603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,9 +1618,11 @@
     <col min="5" max="5" width="14.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.140625" customWidth="1"/>
     <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -428,8 +1644,14 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42552</v>
       </c>
@@ -451,8 +1673,16 @@
       <c r="G2">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>164</v>
+      </c>
+      <c r="I2">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42553</v>
       </c>
@@ -474,8 +1704,16 @@
       <c r="G3">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>165</v>
+      </c>
+      <c r="I3">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42554</v>
       </c>
@@ -497,8 +1735,16 @@
       <c r="G4">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>187</v>
+      </c>
+      <c r="I4">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>46.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42555</v>
       </c>
@@ -520,8 +1766,16 @@
       <c r="G5">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>233</v>
+      </c>
+      <c r="I5">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>58.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>42556</v>
       </c>
@@ -543,8 +1797,16 @@
       <c r="G6">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>277</v>
+      </c>
+      <c r="I6">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>69.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>42557</v>
       </c>
@@ -566,8 +1828,16 @@
       <c r="G7">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>172</v>
+      </c>
+      <c r="I7">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>42558</v>
       </c>
@@ -589,8 +1859,19 @@
       <c r="G8">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>244</v>
+      </c>
+      <c r="I8">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42559</v>
+      </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -609,8 +1890,16 @@
       <c r="G9">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>209</v>
+      </c>
+      <c r="I9">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>52.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>42560</v>
       </c>
@@ -632,8 +1921,16 @@
       <c r="G10">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>229</v>
+      </c>
+      <c r="I10">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>57.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>42561</v>
       </c>
@@ -655,8 +1952,16 @@
       <c r="G11">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>238</v>
+      </c>
+      <c r="I11">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>59.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>42562</v>
       </c>
@@ -678,8 +1983,16 @@
       <c r="G12">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>282</v>
+      </c>
+      <c r="I12">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>70.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>42563</v>
       </c>
@@ -701,8 +2014,16 @@
       <c r="G13">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>225</v>
+      </c>
+      <c r="I13">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>56.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>42564</v>
       </c>
@@ -724,8 +2045,16 @@
       <c r="G14">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>184</v>
+      </c>
+      <c r="I14">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>42565</v>
       </c>
@@ -747,8 +2076,16 @@
       <c r="G15">
         <v>0.25</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>207</v>
+      </c>
+      <c r="I15">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>51.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>42566</v>
       </c>
@@ -770,8 +2107,16 @@
       <c r="G16">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>160</v>
+      </c>
+      <c r="I16">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>42567</v>
       </c>
@@ -793,8 +2138,16 @@
       <c r="G17">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>131</v>
+      </c>
+      <c r="I17">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>65.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>42568</v>
       </c>
@@ -816,8 +2169,16 @@
       <c r="G18">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H18">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>191</v>
+      </c>
+      <c r="I18">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>42569</v>
       </c>
@@ -839,8 +2200,16 @@
       <c r="G19">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>223</v>
+      </c>
+      <c r="I19">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>111.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>42570</v>
       </c>
@@ -862,8 +2231,16 @@
       <c r="G20">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H20">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>207</v>
+      </c>
+      <c r="I20">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>103.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>42571</v>
       </c>
@@ -879,11 +2256,22 @@
       <c r="E21">
         <v>70</v>
       </c>
+      <c r="F21">
+        <v>109</v>
+      </c>
       <c r="G21">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H21">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>113</v>
+      </c>
+      <c r="I21">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>56.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>42572</v>
       </c>
@@ -905,8 +2293,16 @@
       <c r="G22">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H22">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>133</v>
+      </c>
+      <c r="I22">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>66.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>42573</v>
       </c>
@@ -928,8 +2324,16 @@
       <c r="G23">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>187</v>
+      </c>
+      <c r="I23">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>93.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>42574</v>
       </c>
@@ -951,8 +2355,16 @@
       <c r="G24">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>202</v>
+      </c>
+      <c r="I24">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>42575</v>
       </c>
@@ -974,8 +2386,16 @@
       <c r="G25">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H25">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>203</v>
+      </c>
+      <c r="I25">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>101.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>42576</v>
       </c>
@@ -997,8 +2417,16 @@
       <c r="G26">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>269</v>
+      </c>
+      <c r="I26">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>134.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>42577</v>
       </c>
@@ -1020,8 +2448,16 @@
       <c r="G27">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H27">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>305</v>
+      </c>
+      <c r="I27">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>106.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>42578</v>
       </c>
@@ -1043,8 +2479,16 @@
       <c r="G28">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H28">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>172</v>
+      </c>
+      <c r="I28">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>60.199999999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>42579</v>
       </c>
@@ -1066,8 +2510,16 @@
       <c r="G29">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H29">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>159</v>
+      </c>
+      <c r="I29">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>55.65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>42580</v>
       </c>
@@ -1089,8 +2541,16 @@
       <c r="G30">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H30">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>166</v>
+      </c>
+      <c r="I30">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>58.099999999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>42581</v>
       </c>
@@ -1112,8 +2572,16 @@
       <c r="G31">
         <v>0.35</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H31">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>145</v>
+      </c>
+      <c r="I31">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>50.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>42582</v>
       </c>
@@ -1135,11 +2603,37 @@
       <c r="G32">
         <v>0.35</v>
       </c>
+      <c r="H32">
+        <f>Table1[[#This Row],[Lemon]]+Table1[[#This Row],[Orange]]</f>
+        <v>123</v>
+      </c>
+      <c r="I32">
+        <f>Table1[[#This Row],[Price]]*Table1[[#This Row],[Sales]]</f>
+        <v>43.05</v>
+      </c>
+    </row>
+    <row r="37" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H37" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37">
+        <f>SUM(Table1[Revenue])</f>
+        <v>2138</v>
+      </c>
     </row>
   </sheetData>
+  <dataConsolidate/>
+  <conditionalFormatting sqref="E2:E32">
+    <cfRule type="top10" dxfId="0" priority="4" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="3" percent="1" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="2" rank="1"/>
+    <cfRule type="top10" dxfId="3" priority="1" bottom="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>